<commit_message>
made changes to source data
</commit_message>
<xml_diff>
--- a/spreadsheets/decision_treeV2.xlsx
+++ b/spreadsheets/decision_treeV2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="8" r:id="rId1"/>
@@ -1200,7 +1200,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1211,6 +1211,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1408,7 +1411,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="118">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1518,6 +1521,9 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1869,7 +1875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1985,7 +1991,7 @@
       </c>
       <c r="R2">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -2622,7 +2628,7 @@
       </c>
       <c r="O14" s="20" t="str">
         <f ca="1">IF(G$5=2,(VLOOKUP(R$2,P$2:Q$11,2,FALSE)),0)</f>
-        <v>Heal Raises</v>
+        <v>Basic Judo Pose</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -8172,9 +8178,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C1:G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>